<commit_message>
update R values and dates
</commit_message>
<xml_diff>
--- a/dash_app/data/measures_test.xlsx
+++ b/dash_app/data/measures_test.xlsx
@@ -224,8 +224,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -337,53 +341,53 @@
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2" s="1" t="n">
         <v>10000</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="1" t="n">
         <v>150</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="0" t="n">
+      <c r="B6" s="1" t="n">
         <v>4</v>
       </c>
     </row>
@@ -409,113 +413,113 @@
       <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="107.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="107.28"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="3" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="2" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="3" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="3" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="3" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="3" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="4" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="5" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="5" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="4" t="s">
+      <c r="A20" s="5" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="4" t="s">
+      <c r="A21" s="5" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="5" t="s">
+      <c r="A22" s="6" t="s">
         <v>28</v>
       </c>
     </row>
@@ -535,84 +539,72 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="11.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="11.04"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="6" t="n">
+      <c r="B2" s="7" t="n">
         <v>43831</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="C2" s="1" t="n">
         <v>2.25</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="6" t="n">
-        <v>43862</v>
-      </c>
-      <c r="C3" s="0" t="n">
-        <v>2.25</v>
+      <c r="B3" s="7" t="n">
+        <v>43900</v>
+      </c>
+      <c r="C3" s="1" t="n">
+        <v>1.32</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="6" t="n">
-        <v>43900</v>
-      </c>
-      <c r="C4" s="0" t="n">
-        <v>1.32</v>
+      <c r="B4" s="7" t="n">
+        <v>43903</v>
+      </c>
+      <c r="C4" s="1" t="n">
+        <v>1.278</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="6" t="n">
-        <v>43902</v>
-      </c>
-      <c r="C5" s="0" t="n">
-        <v>1.38</v>
+      <c r="B5" s="7" t="n">
+        <v>43908</v>
+      </c>
+      <c r="C5" s="1" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="6" t="n">
-        <v>43903</v>
-      </c>
-      <c r="C6" s="0" t="n">
-        <v>1.278</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="6" t="n">
-        <v>43908</v>
-      </c>
-      <c r="C7" s="0" t="n">
-        <v>0.99</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="6" t="n">
-        <v>43923</v>
-      </c>
-      <c r="C8" s="0" t="n">
-        <v>0.972</v>
-      </c>
-    </row>
+      <c r="B6" s="7" t="n">
+        <v>43928</v>
+      </c>
+      <c r="C6" s="1" t="n">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>